<commit_message>
done full API systemsystem
</commit_message>
<xml_diff>
--- a/web/backend/Python-services/src/data/xlsx/upload/FAMS.xlsx
+++ b/web/backend/Python-services/src/data/xlsx/upload/FAMS.xlsx
@@ -514,67 +514,67 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Phan Lan</t>
+          <t>Lê Hải</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>06/11/2003</t>
+          <t>23/01/2007</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Nam</t>
+          <t>Nữ</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>156 Angela Port, Lake Kathrynmouth</t>
+          <t>2547 Johnathan Port, Zhangton</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>0660727583</t>
+          <t>(176)018-8474x40744</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Hoàng Hiền</t>
+          <t>Vũ Minh</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>Accommodation manager</t>
+          <t>Dance movement psychotherapist</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>5301843837</t>
+          <t>001-614-332-5056</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>Nam</t>
+          <t>Nữ</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>elizabeth53@gmail.com</t>
+          <t>đỗvy13@gmail.com</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>Phạm Quang</t>
+          <t>Đỗ Ngọc</t>
         </is>
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>Dancer</t>
+          <t>Programmer, systems</t>
         </is>
       </c>
       <c r="M2" t="inlineStr">
         <is>
-          <t>050.976.4588x28943</t>
+          <t>(106)376-2466</t>
         </is>
       </c>
       <c r="N2" t="inlineStr">
@@ -584,19 +584,19 @@
       </c>
       <c r="O2" t="inlineStr">
         <is>
-          <t>brandywoods@gmail.com</t>
+          <t>lêhải49@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Phan Vân</t>
+          <t>Phạm Anh</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>25/04/2005</t>
+          <t>30/03/2005</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -606,104 +606,104 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>33409 Jose Common, Johnmouth</t>
+          <t>0956 Dawn Bypass, Gibsonview</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>001-951-053-4964x61336</t>
+          <t>1707448443</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Đỗ Thảo</t>
+          <t>Phạm Lan</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>Acupuncturist</t>
+          <t>Counselling psychologist</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>+1-646-599-8770x555</t>
+          <t>0715384666</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>Nam</t>
+          <t>Nữ</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>thomas37@schroeder-harrison.com</t>
+          <t>phạmvân96@gmail.com</t>
         </is>
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>Đỗ Hiền</t>
+          <t>Phạm Lan</t>
         </is>
       </c>
       <c r="L3" t="inlineStr">
         <is>
-          <t>Engineer, biomedical</t>
+          <t>Recruitment consultant</t>
         </is>
       </c>
       <c r="M3" t="inlineStr">
         <is>
-          <t>001-199-950-8446</t>
+          <t>085-161-3589x1783</t>
         </is>
       </c>
       <c r="N3" t="inlineStr">
         <is>
-          <t>Nữ</t>
+          <t>Nam</t>
         </is>
       </c>
       <c r="O3" t="inlineStr">
         <is>
-          <t>emily76@russell.org</t>
+          <t>trầnhùng93@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Phạm Minh</t>
+          <t>Đặng Vân</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>21/05/2001</t>
+          <t>09/10/2004</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Nam</t>
+          <t>Nữ</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>0019 Adam Village, Whiteheadview</t>
+          <t>93878 Howell Lake, East Joshua</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>(043)820-6425</t>
+          <t>+1-038-257-6114x250</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>Trần Anh</t>
+          <t>Vũ Anh</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>Media planner</t>
+          <t>Runner, broadcasting/film/video</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>929-209-0562x99796</t>
+          <t>093-750-8037</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
@@ -713,22 +713,22 @@
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>cervantessheri@gates.com</t>
+          <t>phantú48@gmail.com</t>
         </is>
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>Trần Anh</t>
+          <t>Đặng Tú</t>
         </is>
       </c>
       <c r="L4" t="inlineStr">
         <is>
-          <t>Doctor, hospital</t>
+          <t>Retail merchandiser</t>
         </is>
       </c>
       <c r="M4" t="inlineStr">
         <is>
-          <t>001-082-339-6812</t>
+          <t>408.206.7420</t>
         </is>
       </c>
       <c r="N4" t="inlineStr">
@@ -738,19 +738,19 @@
       </c>
       <c r="O4" t="inlineStr">
         <is>
-          <t>garygriffith@hotmail.com</t>
+          <t>vũthảo42@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Đỗ Khánh</t>
+          <t>Nguyễn Hải</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>01/09/2005</t>
+          <t>06/04/2007</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -760,129 +760,129 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>75229 David Mission, Andersonville</t>
+          <t>18467 Huang Falls, North Michael</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>431.166.7222</t>
+          <t>7513482676</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>Hoàng Minh</t>
+          <t>Hoàng Khánh</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>Barista</t>
+          <t>Research officer, government</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>534-388-8458x5612</t>
+          <t>759-823-0323x267</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>Nam</t>
+          <t>Nữ</t>
         </is>
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>nramsey@yahoo.com</t>
+          <t>hoàngminh6@gmail.com</t>
         </is>
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>Hoàng Ngọc</t>
+          <t>Trần Khánh</t>
         </is>
       </c>
       <c r="L5" t="inlineStr">
         <is>
-          <t>Astronomer</t>
+          <t>Cartographer</t>
         </is>
       </c>
       <c r="M5" t="inlineStr">
         <is>
-          <t>001-551-865-5032x02359</t>
+          <t>536.193.4019</t>
         </is>
       </c>
       <c r="N5" t="inlineStr">
         <is>
-          <t>Nam</t>
+          <t>Nữ</t>
         </is>
       </c>
       <c r="O5" t="inlineStr">
         <is>
-          <t>reeseamanda@yahoo.com</t>
+          <t>trầnlan82@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Đặng Vy</t>
+          <t>Vũ Thảo</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>31/10/2006</t>
+          <t>17/02/2002</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Nam</t>
+          <t>Nữ</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>78431 Cynthia Junction, Port Kristinastad</t>
+          <t>750 Sandra Garden, East Lawrence</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>536.629.1324x739</t>
+          <t>710.534.2757</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>Phạm Hải</t>
+          <t>Trần Dương</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>Records manager</t>
+          <t>Editor, commissioning</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>+1-194-555-8113x90734</t>
+          <t>754.873.4165x20820</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>Nam</t>
+          <t>Nữ</t>
         </is>
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>elainekirk@gmail.com</t>
+          <t>phạmquang15@gmail.com</t>
         </is>
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>Trần Vân</t>
+          <t>Lê Quang</t>
         </is>
       </c>
       <c r="L6" t="inlineStr">
         <is>
-          <t>Oncologist</t>
+          <t>Scientist, research (medical)</t>
         </is>
       </c>
       <c r="M6" t="inlineStr">
         <is>
-          <t>001-458-647-2189</t>
+          <t>+1-831-782-6108x43088</t>
         </is>
       </c>
       <c r="N6" t="inlineStr">
@@ -892,96 +892,96 @@
       </c>
       <c r="O6" t="inlineStr">
         <is>
-          <t>david57@hotmail.com</t>
+          <t>trầnlinh67@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Trần Linh</t>
+          <t>Bùi Vy</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>12/06/2001</t>
+          <t>08/05/2004</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Nữ</t>
+          <t>Nam</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>32740 Andrew Squares, Briannaside</t>
+          <t>79394 Wood Crossing, New Christineside</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>627-671-6698x7012</t>
+          <t>015-452-2696x3417</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>Trần Châu</t>
+          <t>Bùi Bình</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>Hospital pharmacist</t>
+          <t>Speech and language therapist</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>001-291-006-8090x9164</t>
+          <t>(308)449-1717x045</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>Nam</t>
+          <t>Nữ</t>
         </is>
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>robinsonhector@gmail.com</t>
+          <t>nguyễndương54@gmail.com</t>
         </is>
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>Trần Châu</t>
+          <t>Phạm Khánh</t>
         </is>
       </c>
       <c r="L7" t="inlineStr">
         <is>
-          <t>Economist</t>
+          <t>Recycling officer</t>
         </is>
       </c>
       <c r="M7" t="inlineStr">
         <is>
-          <t>448-040-9643x08801</t>
+          <t>723.224.1571x762</t>
         </is>
       </c>
       <c r="N7" t="inlineStr">
         <is>
-          <t>Nữ</t>
+          <t>Nam</t>
         </is>
       </c>
       <c r="O7" t="inlineStr">
         <is>
-          <t>wesley33@olson-wall.org</t>
+          <t>nguyễnnam91@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Lê Thảo</t>
+          <t>Phạm Minh</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>22/03/2006</t>
+          <t>15/07/2006</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -991,27 +991,27 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>8562 Monica Loop, East Jessica</t>
+          <t>4728 Aaron Orchard, Nicholeville</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>+1-989-951-0820x93981</t>
+          <t>179-225-2744x96909</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>Lê Ngọc</t>
+          <t>Phan Minh</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>Plant breeder/geneticist</t>
+          <t>Editorial assistant</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>596-949-2309</t>
+          <t>(706)667-2307x844</t>
         </is>
       </c>
       <c r="I8" t="inlineStr">
@@ -1021,22 +1021,22 @@
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>dennisyoung@hall.com</t>
+          <t>lêvân92@gmail.com</t>
         </is>
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>Lê Tú</t>
+          <t>Bùi Quang</t>
         </is>
       </c>
       <c r="L8" t="inlineStr">
         <is>
-          <t>Financial planner</t>
+          <t>Garment/textile technologist</t>
         </is>
       </c>
       <c r="M8" t="inlineStr">
         <is>
-          <t>(946)871-5475</t>
+          <t>+1-685-157-9471x086</t>
         </is>
       </c>
       <c r="N8" t="inlineStr">
@@ -1046,49 +1046,49 @@
       </c>
       <c r="O8" t="inlineStr">
         <is>
-          <t>smithpaul@stephens.biz</t>
+          <t>phạmtú89@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Đỗ Thảo</t>
+          <t>Phan Hiền</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>07/08/2005</t>
+          <t>24/03/2006</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Nam</t>
+          <t>Nữ</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>41976 Jones Station, Christineton</t>
+          <t>299 Curtis Way, New Michelleton</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>9163280680</t>
+          <t>626-539-7581x44963</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>Nguyễn Anh</t>
+          <t>Phạm Lan</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>Private music teacher</t>
+          <t>Tax inspector</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>+1-067-908-6688x7131</t>
+          <t>+1-727-373-6434</t>
         </is>
       </c>
       <c r="I9" t="inlineStr">
@@ -1098,44 +1098,44 @@
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>fjenkins@allen.net</t>
+          <t>vũquang20@gmail.com</t>
         </is>
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>Vũ Trang</t>
+          <t>Nguyễn Hiền</t>
         </is>
       </c>
       <c r="L9" t="inlineStr">
         <is>
-          <t>Medical sales representative</t>
+          <t>Facilities manager</t>
         </is>
       </c>
       <c r="M9" t="inlineStr">
         <is>
-          <t>001-665-207-5556x62607</t>
+          <t>567.691.3716x4730</t>
         </is>
       </c>
       <c r="N9" t="inlineStr">
         <is>
-          <t>Nữ</t>
+          <t>Nam</t>
         </is>
       </c>
       <c r="O9" t="inlineStr">
         <is>
-          <t>william09@gmail.com</t>
+          <t>phạmbình65@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Đặng Châu</t>
+          <t>Vũ Phúc</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>27/02/2003</t>
+          <t>30/08/2005</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -1145,52 +1145,52 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>399 Stephanie Pine, West Kevinview</t>
+          <t>353 Jack Overpass, Nancyville</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>001-863-306-5477x544</t>
+          <t>001-641-205-5817x857</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>Bùi Ngọc</t>
+          <t>Hoàng Hải</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>Acupuncturist</t>
+          <t>Journalist, newspaper</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>959.407.6255</t>
+          <t>082-365-4514</t>
         </is>
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>Nữ</t>
+          <t>Nam</t>
         </is>
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>zrobbins@austin.org</t>
+          <t>trầnvy28@gmail.com</t>
         </is>
       </c>
       <c r="K10" t="inlineStr">
         <is>
-          <t>Đặng Thảo</t>
+          <t>Vũ Vân</t>
         </is>
       </c>
       <c r="L10" t="inlineStr">
         <is>
-          <t>IT technical support officer</t>
+          <t>Industrial/product designer</t>
         </is>
       </c>
       <c r="M10" t="inlineStr">
         <is>
-          <t>(307)638-7513x863</t>
+          <t>256-392-2106x912</t>
         </is>
       </c>
       <c r="N10" t="inlineStr">
@@ -1200,49 +1200,49 @@
       </c>
       <c r="O10" t="inlineStr">
         <is>
-          <t>jowens@hotmail.com</t>
+          <t>đỗhiền9@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Trần Hải</t>
+          <t>Trần Châu</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>15/07/2003</t>
+          <t>07/01/2003</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Nam</t>
+          <t>Nữ</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>983 Young Walk, Claireview</t>
+          <t>424 Moran Flats, East Mitchell</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>+1-964-604-3070</t>
+          <t>(642)832-8854x3948</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>Lê Minh</t>
+          <t>Nguyễn Hải</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>Magazine features editor</t>
+          <t>Commercial/residential surveyor</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>499.579.4108x21283</t>
+          <t>375.384.6644x0258</t>
         </is>
       </c>
       <c r="I11" t="inlineStr">
@@ -1252,99 +1252,99 @@
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>xmccarty@hotmail.com</t>
+          <t>trầnhùng88@gmail.com</t>
         </is>
       </c>
       <c r="K11" t="inlineStr">
         <is>
-          <t>Bùi Quang</t>
+          <t>Vũ Quang</t>
         </is>
       </c>
       <c r="L11" t="inlineStr">
         <is>
-          <t>Hydrologist</t>
+          <t>Teacher, special educational needs</t>
         </is>
       </c>
       <c r="M11" t="inlineStr">
         <is>
-          <t>001-833-620-1028</t>
+          <t>001-188-199-2399x959</t>
         </is>
       </c>
       <c r="N11" t="inlineStr">
         <is>
-          <t>Nam</t>
+          <t>Nữ</t>
         </is>
       </c>
       <c r="O11" t="inlineStr">
         <is>
-          <t>ledwards@hotmail.com</t>
+          <t>phanphúc70@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Đỗ Lan</t>
+          <t>Hoàng Nam</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>07/02/2002</t>
+          <t>03/08/2002</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Nam</t>
+          <t>Nữ</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>414 Nicole Ville, Port Edward</t>
+          <t>388 Thomas Corner, Lake Michelleland</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>056-550-4100</t>
+          <t>001-276-251-6853x00094</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>Vũ Quang</t>
+          <t>Vũ Hải</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>Herbalist</t>
+          <t>Administrator, arts</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>631.603.8310x49403</t>
+          <t>777-320-8934x9937</t>
         </is>
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>Nam</t>
+          <t>Nữ</t>
         </is>
       </c>
       <c r="J12" t="inlineStr">
         <is>
-          <t>deborah89@yahoo.com</t>
+          <t>phanvân27@gmail.com</t>
         </is>
       </c>
       <c r="K12" t="inlineStr">
         <is>
-          <t>Hoàng Dương</t>
+          <t>Đặng Anh</t>
         </is>
       </c>
       <c r="L12" t="inlineStr">
         <is>
-          <t>Engineer, control and instrumentation</t>
+          <t>Archivist</t>
         </is>
       </c>
       <c r="M12" t="inlineStr">
         <is>
-          <t>(339)566-4016x7202</t>
+          <t>001-235-820-8505x2189</t>
         </is>
       </c>
       <c r="N12" t="inlineStr">
@@ -1354,74 +1354,74 @@
       </c>
       <c r="O12" t="inlineStr">
         <is>
-          <t>lindaleblanc@alvarez-alexander.com</t>
+          <t>đỗlan26@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Trần Anh</t>
+          <t>Phan Vy</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>02/07/2001</t>
+          <t>29/10/2004</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Nữ</t>
+          <t>Nam</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>8346 Booth Creek, Whiteville</t>
+          <t>34521 Jose Glens, West Joefurt</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>821.740.9296x8709</t>
+          <t>400-662-3451x557</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>Nguyễn Lan</t>
+          <t>Nguyễn Linh</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>Magazine features editor</t>
+          <t>Surveyor, quantity</t>
         </is>
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>+1-562-637-5307x63213</t>
+          <t>+1-127-550-7816x42872</t>
         </is>
       </c>
       <c r="I13" t="inlineStr">
         <is>
-          <t>Nữ</t>
+          <t>Nam</t>
         </is>
       </c>
       <c r="J13" t="inlineStr">
         <is>
-          <t>gturner@adams.com</t>
+          <t>hoànganh60@gmail.com</t>
         </is>
       </c>
       <c r="K13" t="inlineStr">
         <is>
-          <t>Đỗ Linh</t>
+          <t>Trần Tú</t>
         </is>
       </c>
       <c r="L13" t="inlineStr">
         <is>
-          <t>Sports coach</t>
+          <t>Garment/textile technologist</t>
         </is>
       </c>
       <c r="M13" t="inlineStr">
         <is>
-          <t>001-177-166-1580x207</t>
+          <t>696-209-4760</t>
         </is>
       </c>
       <c r="N13" t="inlineStr">
@@ -1431,96 +1431,96 @@
       </c>
       <c r="O13" t="inlineStr">
         <is>
-          <t>cynthiafoster@gmail.com</t>
+          <t>lêanh56@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Vũ Quang</t>
+          <t>Hoàng Nam</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>19/02/2006</t>
+          <t>17/11/2006</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Nam</t>
+          <t>Nữ</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>2107 Holland Course, Wendyside</t>
+          <t>303 Mcdonald Stream, South Cindy</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>001-592-730-3015x4169</t>
+          <t>2508742755</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>Đỗ Anh</t>
+          <t>Đặng Bình</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>Industrial/product designer</t>
+          <t>Barista</t>
         </is>
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>001-650-567-8555x935</t>
+          <t>(673)209-5719x01308</t>
         </is>
       </c>
       <c r="I14" t="inlineStr">
         <is>
-          <t>Nam</t>
+          <t>Nữ</t>
         </is>
       </c>
       <c r="J14" t="inlineStr">
         <is>
-          <t>melissagomez@yahoo.com</t>
+          <t>nguyễnnam63@gmail.com</t>
         </is>
       </c>
       <c r="K14" t="inlineStr">
         <is>
-          <t>Đỗ Phúc</t>
+          <t>Phạm Khánh</t>
         </is>
       </c>
       <c r="L14" t="inlineStr">
         <is>
-          <t>Furniture designer</t>
+          <t>Teaching laboratory technician</t>
         </is>
       </c>
       <c r="M14" t="inlineStr">
         <is>
-          <t>001-090-258-3865</t>
+          <t>(306)124-1745x397</t>
         </is>
       </c>
       <c r="N14" t="inlineStr">
         <is>
-          <t>Nữ</t>
+          <t>Nam</t>
         </is>
       </c>
       <c r="O14" t="inlineStr">
         <is>
-          <t>morgan61@whitney.com</t>
+          <t>vũphúc70@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Phan Châu</t>
+          <t>Lê Khánh</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>16/02/2005</t>
+          <t>23/04/2007</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
@@ -1530,74 +1530,74 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>199 Solomon Viaduct, Hallton</t>
+          <t>311 Miller Place, Gregoryland</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>275.431.3362</t>
+          <t>3191633569</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>Đặng Hải</t>
+          <t>Vũ Linh</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>Community pharmacist</t>
+          <t>Television camera operator</t>
         </is>
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>268.945.5195</t>
+          <t>+1-147-171-9487</t>
         </is>
       </c>
       <c r="I15" t="inlineStr">
         <is>
-          <t>Nam</t>
+          <t>Nữ</t>
         </is>
       </c>
       <c r="J15" t="inlineStr">
         <is>
-          <t>melissahorton@yahoo.com</t>
+          <t>trầnlinh33@gmail.com</t>
         </is>
       </c>
       <c r="K15" t="inlineStr">
         <is>
-          <t>Phạm Vân</t>
+          <t>Lê Hiền</t>
         </is>
       </c>
       <c r="L15" t="inlineStr">
         <is>
-          <t>Education officer, museum</t>
+          <t>Scientist, research (life sciences)</t>
         </is>
       </c>
       <c r="M15" t="inlineStr">
         <is>
-          <t>+1-839-656-6687x73038</t>
+          <t>(221)668-3953</t>
         </is>
       </c>
       <c r="N15" t="inlineStr">
         <is>
-          <t>Nam</t>
+          <t>Nữ</t>
         </is>
       </c>
       <c r="O15" t="inlineStr">
         <is>
-          <t>lukepalmer@huffman-harris.com</t>
+          <t>nguyễnminh84@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Đỗ Vân</t>
+          <t>Đặng Anh</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>01/04/2004</t>
+          <t>18/08/2001</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
@@ -1607,104 +1607,104 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>591 Aguirre Fields, South Erica</t>
+          <t>43701 Brandon Run, Sandrabury</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>+1-749-205-0998x3237</t>
+          <t>+1-640-520-6415x4404</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>Nguyễn Hiền</t>
+          <t>Bùi Phúc</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>Visual merchandiser</t>
+          <t>Surveyor, commercial/residential</t>
         </is>
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>+1-433-801-3739</t>
+          <t>969.382.2391x3838</t>
         </is>
       </c>
       <c r="I16" t="inlineStr">
         <is>
-          <t>Nam</t>
+          <t>Nữ</t>
         </is>
       </c>
       <c r="J16" t="inlineStr">
         <is>
-          <t>rbell@montoya.biz</t>
+          <t>đặngngọc53@gmail.com</t>
         </is>
       </c>
       <c r="K16" t="inlineStr">
         <is>
-          <t>Phạm Quang</t>
+          <t>Phan Trang</t>
         </is>
       </c>
       <c r="L16" t="inlineStr">
         <is>
-          <t>Community education officer</t>
+          <t>Operations geologist</t>
         </is>
       </c>
       <c r="M16" t="inlineStr">
         <is>
-          <t>+1-470-696-1731x800</t>
+          <t>587.320.7002x937</t>
         </is>
       </c>
       <c r="N16" t="inlineStr">
         <is>
-          <t>Nữ</t>
+          <t>Nam</t>
         </is>
       </c>
       <c r="O16" t="inlineStr">
         <is>
-          <t>jakegay@yahoo.com</t>
+          <t>đỗquang68@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Đỗ Tú</t>
+          <t>Đặng Hùng</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>07/02/2006</t>
+          <t>08/08/2001</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Nam</t>
+          <t>Nữ</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>1308 Kevin Lights, Mirandastad</t>
+          <t>8501 Wilson Fields, Phillipsfurt</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>667-986-4146</t>
+          <t>001-353-495-0798</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>Đỗ Tú</t>
+          <t>Phạm Trang</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>Barista</t>
+          <t>Public relations officer</t>
         </is>
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>9887088305</t>
+          <t>+1-912-932-0699x3675</t>
         </is>
       </c>
       <c r="I17" t="inlineStr">
@@ -1714,22 +1714,22 @@
       </c>
       <c r="J17" t="inlineStr">
         <is>
-          <t>dustin32@armstrong.info</t>
+          <t>hoàngvy17@gmail.com</t>
         </is>
       </c>
       <c r="K17" t="inlineStr">
         <is>
-          <t>Lê Hải</t>
+          <t>Phạm Anh</t>
         </is>
       </c>
       <c r="L17" t="inlineStr">
         <is>
-          <t>Doctor, general practice</t>
+          <t>Sports development officer</t>
         </is>
       </c>
       <c r="M17" t="inlineStr">
         <is>
-          <t>828.051.4254</t>
+          <t>223-258-4554x177</t>
         </is>
       </c>
       <c r="N17" t="inlineStr">
@@ -1739,126 +1739,126 @@
       </c>
       <c r="O17" t="inlineStr">
         <is>
-          <t>patriciabryant@yahoo.com</t>
+          <t>nguyễnvy15@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Lê Hải</t>
+          <t>Vũ Bình</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>13/08/2006</t>
+          <t>07/08/2003</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Nam</t>
+          <t>Nữ</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>0229 Lambert Street, Carolchester</t>
+          <t>501 Tyler Motorway, Lake Danielmouth</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>+1-892-275-5274x22980</t>
+          <t>(651)502-9036</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>Bùi Khánh</t>
+          <t>Nguyễn Vân</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>Health visitor</t>
+          <t>Information systems manager</t>
         </is>
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>661-378-9092x70371</t>
+          <t>933-710-9460</t>
         </is>
       </c>
       <c r="I18" t="inlineStr">
         <is>
-          <t>Nữ</t>
+          <t>Nam</t>
         </is>
       </c>
       <c r="J18" t="inlineStr">
         <is>
-          <t>ddavis@james.net</t>
+          <t>bùilinh66@gmail.com</t>
         </is>
       </c>
       <c r="K18" t="inlineStr">
         <is>
-          <t>Hoàng Khánh</t>
+          <t>Đỗ Trang</t>
         </is>
       </c>
       <c r="L18" t="inlineStr">
         <is>
-          <t>IT technical support officer</t>
+          <t>Furniture conservator/restorer</t>
         </is>
       </c>
       <c r="M18" t="inlineStr">
         <is>
-          <t>001-379-863-8361x60979</t>
+          <t>116-019-5715x31952</t>
         </is>
       </c>
       <c r="N18" t="inlineStr">
         <is>
-          <t>Nam</t>
+          <t>Nữ</t>
         </is>
       </c>
       <c r="O18" t="inlineStr">
         <is>
-          <t>millerbrandy@hall.net</t>
+          <t>trầnquang41@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Phạm Dương</t>
+          <t>Đỗ Hải</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>16/06/2000</t>
+          <t>27/12/2001</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Nữ</t>
+          <t>Nam</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>679 Clayton Overpass, South Jessicaville</t>
+          <t>2388 Matthew Plains, Knappfurt</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>(378)576-5763x274</t>
+          <t>5032597647</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>Bùi Hiền</t>
+          <t>Phạm Bình</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>Archaeologist</t>
+          <t>Records manager</t>
         </is>
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>+1-211-502-7557x29840</t>
+          <t>083-301-4467</t>
         </is>
       </c>
       <c r="I19" t="inlineStr">
@@ -1868,22 +1868,22 @@
       </c>
       <c r="J19" t="inlineStr">
         <is>
-          <t>joshuamullen@gibson-good.net</t>
+          <t>nguyễnminh48@gmail.com</t>
         </is>
       </c>
       <c r="K19" t="inlineStr">
         <is>
-          <t>Nguyễn Bình</t>
+          <t>Phan Phúc</t>
         </is>
       </c>
       <c r="L19" t="inlineStr">
         <is>
-          <t>Paramedic</t>
+          <t>Research scientist (maths)</t>
         </is>
       </c>
       <c r="M19" t="inlineStr">
         <is>
-          <t>+1-642-530-7153x30820</t>
+          <t>001-199-690-4025x0756</t>
         </is>
       </c>
       <c r="N19" t="inlineStr">
@@ -1893,19 +1893,19 @@
       </c>
       <c r="O19" t="inlineStr">
         <is>
-          <t>nicholasrobinson@yahoo.com</t>
+          <t>bùichâu89@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Lê Khánh</t>
+          <t>Bùi Quang</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>10/03/2007</t>
+          <t>27/07/2000</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
@@ -1915,27 +1915,27 @@
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>89130 Megan Rapids, Lake Susan</t>
+          <t>68326 Gonzalez Heights, Sarahburgh</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>598.860.8031</t>
+          <t>(955)035-6896</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>Hoàng Dương</t>
+          <t>Phan Hải</t>
         </is>
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>Programmer, multimedia</t>
+          <t>Private music teacher</t>
         </is>
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>(389)257-8736</t>
+          <t>001-568-743-5003x63593</t>
         </is>
       </c>
       <c r="I20" t="inlineStr">
@@ -1945,44 +1945,44 @@
       </c>
       <c r="J20" t="inlineStr">
         <is>
-          <t>lcrawford@gmail.com</t>
+          <t>trầnbình7@gmail.com</t>
         </is>
       </c>
       <c r="K20" t="inlineStr">
         <is>
-          <t>Bùi Trang</t>
+          <t>Trần Trang</t>
         </is>
       </c>
       <c r="L20" t="inlineStr">
         <is>
-          <t>Financial planner</t>
+          <t>Manufacturing engineer</t>
         </is>
       </c>
       <c r="M20" t="inlineStr">
         <is>
-          <t>808-589-2381</t>
+          <t>(225)192-3757</t>
         </is>
       </c>
       <c r="N20" t="inlineStr">
         <is>
-          <t>Nữ</t>
+          <t>Nam</t>
         </is>
       </c>
       <c r="O20" t="inlineStr">
         <is>
-          <t>bethmcdaniel@ryan.com</t>
+          <t>hoàngnam35@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Hoàng Vân</t>
+          <t>Trần Châu</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>05/06/2004</t>
+          <t>23/09/2002</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
@@ -1992,27 +1992,27 @@
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>9211 Robertson Forest, Fletcherside</t>
+          <t>92336 Fisher Run, South Kristen</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>+1-065-411-6510x77627</t>
+          <t>(150)682-2387x0232</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>Đặng Vy</t>
+          <t>Trần Vân</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>Therapist, occupational</t>
+          <t>Broadcast presenter</t>
         </is>
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>001-654-762-3303x4612</t>
+          <t>333-338-3633</t>
         </is>
       </c>
       <c r="I21" t="inlineStr">
@@ -2022,22 +2022,22 @@
       </c>
       <c r="J21" t="inlineStr">
         <is>
-          <t>cscott@diaz.info</t>
+          <t>lênam89@gmail.com</t>
         </is>
       </c>
       <c r="K21" t="inlineStr">
         <is>
-          <t>Đỗ Hùng</t>
+          <t>Đỗ Khánh</t>
         </is>
       </c>
       <c r="L21" t="inlineStr">
         <is>
-          <t>Biomedical engineer</t>
+          <t>Exercise physiologist</t>
         </is>
       </c>
       <c r="M21" t="inlineStr">
         <is>
-          <t>001-760-392-2269x61148</t>
+          <t>+1-369-188-0062x75706</t>
         </is>
       </c>
       <c r="N21" t="inlineStr">
@@ -2047,7 +2047,7 @@
       </c>
       <c r="O21" t="inlineStr">
         <is>
-          <t>ejones@gomez.biz</t>
+          <t>hoàngdương6@gmail.com</t>
         </is>
       </c>
     </row>
@@ -2062,7 +2062,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I21"/>
+  <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2120,12 +2120,12 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Vũ Ngọc</t>
+          <t>Lê Ngọc</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>25/02/1998</t>
+          <t>25/06/1992</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -2135,42 +2135,42 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>7894 Baldwin Views, West Robin</t>
+          <t>178 Snyder Skyway, Jeffersonport</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>540.729.2013x563</t>
+          <t>001-190-666-1643</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>vũngọc41@gmail.com</t>
+          <t>lêngọc15@gmail.com</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>Sales executive</t>
+          <t>Research scientist (life sciences)</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>Tiến sĩ</t>
+          <t>Thạc sĩ</t>
         </is>
       </c>
       <c r="I2" t="n">
-        <v>17</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Vũ Minh</t>
+          <t>Phan Linh</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>17/04/1988</t>
+          <t>21/06/1987</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -2180,42 +2180,42 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>573 Erica Road, Port Kelly</t>
+          <t>28349 Jeremy Pine, Aliciaburgh</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>853.069.1260x246</t>
+          <t>+1-133-146-4815x81070</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>vũminh75@gmail.com</t>
+          <t>phanlinh29@gmail.com</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>Building control surveyor</t>
+          <t>Doctor, hospital</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>Tiến sĩ</t>
+          <t>Cử nhân</t>
         </is>
       </c>
       <c r="I3" t="n">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Vũ Ngọc</t>
+          <t>Trần Khánh</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>25/12/1999</t>
+          <t>23/10/1995</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -2225,42 +2225,42 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>24729 Pratt Street, Tuckerville</t>
+          <t>450 Dodson Place, Smithbury</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>+1-742-225-4021x88817</t>
+          <t>(074)218-0224x3816</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>vũngọc12@gmail.com</t>
+          <t>trầnkhánh28@gmail.com</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>Geochemist</t>
+          <t>Proofreader</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>Thạc sĩ</t>
+          <t>Tiến sĩ</t>
         </is>
       </c>
       <c r="I4" t="n">
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Vũ Quang</t>
+          <t>Trần Trang</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>16/03/1988</t>
+          <t>03/01/1992</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -2270,751 +2270,76 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>91849 William Garden, North Franklin</t>
+          <t>7692 Christian Drive, East Kevin</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>109.798.8627</t>
+          <t>+1-728-012-8475</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>vũquang74@gmail.com</t>
+          <t>trầntrang87@gmail.com</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>Civil Service administrator</t>
+          <t>Chief Marketing Officer</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>Cử nhân</t>
+          <t>Tiến sĩ</t>
         </is>
       </c>
       <c r="I5" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Trần Châu</t>
+          <t>Vũ Minh</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>17/05/1992</t>
+          <t>13/12/1996</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Nam</t>
+          <t>Nữ</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>036 Katherine Branch, North Sandrabury</t>
+          <t>07857 Rojas Streets, Andersenmouth</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>(564)847-9088x1409</t>
+          <t>(784)532-8624</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>trầnchâu42@gmail.com</t>
+          <t>vũminh7@gmail.com</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>Teacher, music</t>
+          <t>Broadcast presenter</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>Tiến sĩ</t>
+          <t>Cử nhân</t>
         </is>
       </c>
       <c r="I6" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>Vũ Hiền</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>28/04/1988</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>Nữ</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>34232 Krystal Terrace, Lake Lydiafort</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>+1-287-729-4059</t>
-        </is>
-      </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>vũhiền94@gmail.com</t>
-        </is>
-      </c>
-      <c r="G7" t="inlineStr">
-        <is>
-          <t>Web designer</t>
-        </is>
-      </c>
-      <c r="H7" t="inlineStr">
-        <is>
-          <t>Thạc sĩ</t>
-        </is>
-      </c>
-      <c r="I7" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>Đặng Hải</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>16/10/1985</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>Nữ</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>295 Riddle Mission, Westview</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>978-199-8647x9210</t>
-        </is>
-      </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>đặnghải41@gmail.com</t>
-        </is>
-      </c>
-      <c r="G8" t="inlineStr">
-        <is>
-          <t>Insurance risk surveyor</t>
-        </is>
-      </c>
-      <c r="H8" t="inlineStr">
-        <is>
-          <t>Thạc sĩ</t>
-        </is>
-      </c>
-      <c r="I8" t="n">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>Hoàng Anh</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>31/12/1984</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>Nữ</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>53346 Mendez Drives, Amandaview</t>
-        </is>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>+1-088-581-1848</t>
-        </is>
-      </c>
-      <c r="F9" t="inlineStr">
-        <is>
-          <t>hoànganh68@gmail.com</t>
-        </is>
-      </c>
-      <c r="G9" t="inlineStr">
-        <is>
-          <t>Homeopath</t>
-        </is>
-      </c>
-      <c r="H9" t="inlineStr">
-        <is>
-          <t>Cử nhân</t>
-        </is>
-      </c>
-      <c r="I9" t="n">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>Đỗ Hải</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>14/10/1985</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>Nam</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>147 Nancy Port, Chavezburgh</t>
-        </is>
-      </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>(171)538-7162x37117</t>
-        </is>
-      </c>
-      <c r="F10" t="inlineStr">
-        <is>
-          <t>đỗhải89@gmail.com</t>
-        </is>
-      </c>
-      <c r="G10" t="inlineStr">
-        <is>
-          <t>Market researcher</t>
-        </is>
-      </c>
-      <c r="H10" t="inlineStr">
-        <is>
-          <t>Tiến sĩ</t>
-        </is>
-      </c>
-      <c r="I10" t="n">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>Vũ Ngọc</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>29/07/1992</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>Nữ</t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>296 Holmes Roads, New Brian</t>
-        </is>
-      </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>+1-034-813-0781x4865</t>
-        </is>
-      </c>
-      <c r="F11" t="inlineStr">
-        <is>
-          <t>vũngọc59@gmail.com</t>
-        </is>
-      </c>
-      <c r="G11" t="inlineStr">
-        <is>
-          <t>Intelligence analyst</t>
-        </is>
-      </c>
-      <c r="H11" t="inlineStr">
-        <is>
-          <t>Thạc sĩ</t>
-        </is>
-      </c>
-      <c r="I11" t="n">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>Đỗ Hiền</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>05/01/1995</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>Nữ</t>
-        </is>
-      </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>117 Victoria Glens, Port Kimberly</t>
-        </is>
-      </c>
-      <c r="E12" t="inlineStr">
-        <is>
-          <t>333-013-5838x4948</t>
-        </is>
-      </c>
-      <c r="F12" t="inlineStr">
-        <is>
-          <t>đỗhiền28@gmail.com</t>
-        </is>
-      </c>
-      <c r="G12" t="inlineStr">
-        <is>
-          <t>Loss adjuster, chartered</t>
-        </is>
-      </c>
-      <c r="H12" t="inlineStr">
-        <is>
-          <t>Thạc sĩ</t>
-        </is>
-      </c>
-      <c r="I12" t="n">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>Đỗ Bình</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>21/10/1989</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>Nam</t>
-        </is>
-      </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>0740 James Burg, South William</t>
-        </is>
-      </c>
-      <c r="E13" t="inlineStr">
-        <is>
-          <t>001-953-452-9388x3046</t>
-        </is>
-      </c>
-      <c r="F13" t="inlineStr">
-        <is>
-          <t>đỗbình1@gmail.com</t>
-        </is>
-      </c>
-      <c r="G13" t="inlineStr">
-        <is>
-          <t>Merchant navy officer</t>
-        </is>
-      </c>
-      <c r="H13" t="inlineStr">
-        <is>
-          <t>Thạc sĩ</t>
-        </is>
-      </c>
-      <c r="I13" t="n">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>Phan Bình</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>07/02/1988</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>Nam</t>
-        </is>
-      </c>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t>9595 Lawrence Ferry, West Jorge</t>
-        </is>
-      </c>
-      <c r="E14" t="inlineStr">
-        <is>
-          <t>001-855-651-8004x6328</t>
-        </is>
-      </c>
-      <c r="F14" t="inlineStr">
-        <is>
-          <t>phanbình7@gmail.com</t>
-        </is>
-      </c>
-      <c r="G14" t="inlineStr">
-        <is>
-          <t>Copywriter, advertising</t>
-        </is>
-      </c>
-      <c r="H14" t="inlineStr">
-        <is>
-          <t>Thạc sĩ</t>
-        </is>
-      </c>
-      <c r="I14" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>Đặng Linh</t>
-        </is>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>18/08/1993</t>
-        </is>
-      </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>Nữ</t>
-        </is>
-      </c>
-      <c r="D15" t="inlineStr">
-        <is>
-          <t>63213 Winters Expressway, Port Johnside</t>
-        </is>
-      </c>
-      <c r="E15" t="inlineStr">
-        <is>
-          <t>092-902-4275x21080</t>
-        </is>
-      </c>
-      <c r="F15" t="inlineStr">
-        <is>
-          <t>đặnglinh27@gmail.com</t>
-        </is>
-      </c>
-      <c r="G15" t="inlineStr">
-        <is>
-          <t>Quantity surveyor</t>
-        </is>
-      </c>
-      <c r="H15" t="inlineStr">
-        <is>
-          <t>Thạc sĩ</t>
-        </is>
-      </c>
-      <c r="I15" t="n">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>Hoàng Hiền</t>
-        </is>
-      </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>25/07/1996</t>
-        </is>
-      </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>Nam</t>
-        </is>
-      </c>
-      <c r="D16" t="inlineStr">
-        <is>
-          <t>27081 Shannon Spring, East Nicole</t>
-        </is>
-      </c>
-      <c r="E16" t="inlineStr">
-        <is>
-          <t>9996574642</t>
-        </is>
-      </c>
-      <c r="F16" t="inlineStr">
-        <is>
-          <t>hoànghiền71@gmail.com</t>
-        </is>
-      </c>
-      <c r="G16" t="inlineStr">
-        <is>
-          <t>International aid/development worker</t>
-        </is>
-      </c>
-      <c r="H16" t="inlineStr">
-        <is>
-          <t>Cử nhân</t>
-        </is>
-      </c>
-      <c r="I16" t="n">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>Phạm Hùng</t>
-        </is>
-      </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>25/12/1993</t>
-        </is>
-      </c>
-      <c r="C17" t="inlineStr">
-        <is>
-          <t>Nữ</t>
-        </is>
-      </c>
-      <c r="D17" t="inlineStr">
-        <is>
-          <t>390 Dixon Ridge, Anthonyberg</t>
-        </is>
-      </c>
-      <c r="E17" t="inlineStr">
-        <is>
-          <t>6797555531</t>
-        </is>
-      </c>
-      <c r="F17" t="inlineStr">
-        <is>
-          <t>phạmhùng44@gmail.com</t>
-        </is>
-      </c>
-      <c r="G17" t="inlineStr">
-        <is>
-          <t>Psychotherapist, child</t>
-        </is>
-      </c>
-      <c r="H17" t="inlineStr">
-        <is>
-          <t>Tiến sĩ</t>
-        </is>
-      </c>
-      <c r="I17" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>Vũ Quang</t>
-        </is>
-      </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>15/09/1993</t>
-        </is>
-      </c>
-      <c r="C18" t="inlineStr">
-        <is>
-          <t>Nam</t>
-        </is>
-      </c>
-      <c r="D18" t="inlineStr">
-        <is>
-          <t>1266 Derrick Row, Ericside</t>
-        </is>
-      </c>
-      <c r="E18" t="inlineStr">
-        <is>
-          <t>715.027.8934x4504</t>
-        </is>
-      </c>
-      <c r="F18" t="inlineStr">
-        <is>
-          <t>vũquang96@gmail.com</t>
-        </is>
-      </c>
-      <c r="G18" t="inlineStr">
-        <is>
-          <t>Sales executive</t>
-        </is>
-      </c>
-      <c r="H18" t="inlineStr">
-        <is>
-          <t>Tiến sĩ</t>
-        </is>
-      </c>
-      <c r="I18" t="n">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>Hoàng Tú</t>
-        </is>
-      </c>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>07/11/1987</t>
-        </is>
-      </c>
-      <c r="C19" t="inlineStr">
-        <is>
-          <t>Nam</t>
-        </is>
-      </c>
-      <c r="D19" t="inlineStr">
-        <is>
-          <t>28898 Christian Cliffs, South Edwardstad</t>
-        </is>
-      </c>
-      <c r="E19" t="inlineStr">
-        <is>
-          <t>+1-123-530-7016x46087</t>
-        </is>
-      </c>
-      <c r="F19" t="inlineStr">
-        <is>
-          <t>hoàngtú18@gmail.com</t>
-        </is>
-      </c>
-      <c r="G19" t="inlineStr">
-        <is>
-          <t>Oceanographer</t>
-        </is>
-      </c>
-      <c r="H19" t="inlineStr">
-        <is>
-          <t>Tiến sĩ</t>
-        </is>
-      </c>
-      <c r="I19" t="n">
         <v>8</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>Nguyễn Hiền</t>
-        </is>
-      </c>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>15/01/1991</t>
-        </is>
-      </c>
-      <c r="C20" t="inlineStr">
-        <is>
-          <t>Nam</t>
-        </is>
-      </c>
-      <c r="D20" t="inlineStr">
-        <is>
-          <t>53519 Santos Shores, New Elizabethbury</t>
-        </is>
-      </c>
-      <c r="E20" t="inlineStr">
-        <is>
-          <t>+1-316-049-8236x6486</t>
-        </is>
-      </c>
-      <c r="F20" t="inlineStr">
-        <is>
-          <t>nguyễnhiền54@gmail.com</t>
-        </is>
-      </c>
-      <c r="G20" t="inlineStr">
-        <is>
-          <t>Applications developer</t>
-        </is>
-      </c>
-      <c r="H20" t="inlineStr">
-        <is>
-          <t>Cử nhân</t>
-        </is>
-      </c>
-      <c r="I20" t="n">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="inlineStr">
-        <is>
-          <t>Trần Linh</t>
-        </is>
-      </c>
-      <c r="B21" t="inlineStr">
-        <is>
-          <t>12/12/1994</t>
-        </is>
-      </c>
-      <c r="C21" t="inlineStr">
-        <is>
-          <t>Nam</t>
-        </is>
-      </c>
-      <c r="D21" t="inlineStr">
-        <is>
-          <t>490 Kristen Court, Bradleyborough</t>
-        </is>
-      </c>
-      <c r="E21" t="inlineStr">
-        <is>
-          <t>+1-221-009-9121x0827</t>
-        </is>
-      </c>
-      <c r="F21" t="inlineStr">
-        <is>
-          <t>trầnlinh57@gmail.com</t>
-        </is>
-      </c>
-      <c r="G21" t="inlineStr">
-        <is>
-          <t>Secretary/administrator</t>
-        </is>
-      </c>
-      <c r="H21" t="inlineStr">
-        <is>
-          <t>Cử nhân</t>
-        </is>
-      </c>
-      <c r="I21" t="n">
-        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update scheduel & API class view
</commit_message>
<xml_diff>
--- a/web/backend/Python-services/src/data/xlsx/upload/FAMS.xlsx
+++ b/web/backend/Python-services/src/data/xlsx/upload/FAMS.xlsx
@@ -514,42 +514,42 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Lê Hải</t>
+          <t>Nguyễn Văn A</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>23/01/2007</t>
+          <t>01/01/2010</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Nữ</t>
+          <t>Nam</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>2547 Johnathan Port, Zhangton</t>
+          <t>Số 1 Đường Nguyễn Huệ, TP Huế</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>(176)018-8474x40744</t>
+          <t>0901234100</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Vũ Minh</t>
+          <t>Phạm Thị A</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>Dance movement psychotherapist</t>
+          <t>Công nhân</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>001-614-332-5056</t>
+          <t>091234510</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
@@ -559,44 +559,44 @@
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>đỗvy13@gmail.com</t>
+          <t>ph10@gmail.com</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>Đỗ Ngọc</t>
+          <t>Phạm Thị B</t>
         </is>
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>Programmer, systems</t>
+          <t>Kỹ sư</t>
         </is>
       </c>
       <c r="M2" t="inlineStr">
         <is>
-          <t>(106)376-2466</t>
+          <t>098765410</t>
         </is>
       </c>
       <c r="N2" t="inlineStr">
         <is>
-          <t>Nữ</t>
+          <t>Nam</t>
         </is>
       </c>
       <c r="O2" t="inlineStr">
         <is>
-          <t>lêhải49@gmail.com</t>
+          <t>ph20@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Phạm Anh</t>
+          <t>Nguyễn Văn B</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>30/03/2005</t>
+          <t>01/01/2011</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -606,129 +606,129 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>0956 Dawn Bypass, Gibsonview</t>
+          <t>Số 2 Đường Nguyễn Huệ, TP Huế</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>1707448443</t>
+          <t>0901234101</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Phạm Lan</t>
+          <t>Phạm Thị C</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>Counselling psychologist</t>
+          <t>Nhân viên văn phòng</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>0715384666</t>
+          <t>091234511</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>Nữ</t>
+          <t>Nam</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>phạmvân96@gmail.com</t>
+          <t>ph11@gmail.com</t>
         </is>
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>Phạm Lan</t>
+          <t>Phạm Thị D</t>
         </is>
       </c>
       <c r="L3" t="inlineStr">
         <is>
-          <t>Recruitment consultant</t>
+          <t>Công nhân</t>
         </is>
       </c>
       <c r="M3" t="inlineStr">
         <is>
-          <t>085-161-3589x1783</t>
+          <t>098765411</t>
         </is>
       </c>
       <c r="N3" t="inlineStr">
         <is>
-          <t>Nam</t>
+          <t>Nữ</t>
         </is>
       </c>
       <c r="O3" t="inlineStr">
         <is>
-          <t>trầnhùng93@gmail.com</t>
+          <t>ph21@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Đặng Vân</t>
+          <t>Nguyễn Văn C</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>09/10/2004</t>
+          <t>01/01/2012</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Nữ</t>
+          <t>Nam</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>93878 Howell Lake, East Joshua</t>
+          <t>Số 3 Đường Nguyễn Huệ, TP Huế</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>+1-038-257-6114x250</t>
+          <t>0901234102</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>Vũ Anh</t>
+          <t>Phạm Thị E</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>Runner, broadcasting/film/video</t>
+          <t>Bác sĩ</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>093-750-8037</t>
+          <t>091234512</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>Nam</t>
+          <t>Nữ</t>
         </is>
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>phantú48@gmail.com</t>
+          <t>ph12@gmail.com</t>
         </is>
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>Đặng Tú</t>
+          <t>Phạm Thị F</t>
         </is>
       </c>
       <c r="L4" t="inlineStr">
         <is>
-          <t>Retail merchandiser</t>
+          <t>Giáo viên</t>
         </is>
       </c>
       <c r="M4" t="inlineStr">
         <is>
-          <t>408.206.7420</t>
+          <t>098765412</t>
         </is>
       </c>
       <c r="N4" t="inlineStr">
@@ -738,74 +738,74 @@
       </c>
       <c r="O4" t="inlineStr">
         <is>
-          <t>vũthảo42@gmail.com</t>
+          <t>ph22@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Nguyễn Hải</t>
+          <t>Nguyễn Văn D</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>06/04/2007</t>
+          <t>01/01/2013</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Nam</t>
+          <t>Nữ</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>18467 Huang Falls, North Michael</t>
+          <t>Số 4 Đường Nguyễn Huệ, TP Huế</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>7513482676</t>
+          <t>0901234103</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>Hoàng Khánh</t>
+          <t>Phạm Thị G</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>Research officer, government</t>
+          <t>Giáo viên</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>759-823-0323x267</t>
+          <t>091234513</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>Nữ</t>
+          <t>Nam</t>
         </is>
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>hoàngminh6@gmail.com</t>
+          <t>ph13@gmail.com</t>
         </is>
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>Trần Khánh</t>
+          <t>Phạm Thị H</t>
         </is>
       </c>
       <c r="L5" t="inlineStr">
         <is>
-          <t>Cartographer</t>
+          <t>Bác sĩ</t>
         </is>
       </c>
       <c r="M5" t="inlineStr">
         <is>
-          <t>536.193.4019</t>
+          <t>098765413</t>
         </is>
       </c>
       <c r="N5" t="inlineStr">
@@ -815,49 +815,49 @@
       </c>
       <c r="O5" t="inlineStr">
         <is>
-          <t>trầnlan82@gmail.com</t>
+          <t>ph23@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Vũ Thảo</t>
+          <t>Nguyễn Văn E</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>17/02/2002</t>
+          <t>01/01/2014</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Nữ</t>
+          <t>Nam</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>750 Sandra Garden, East Lawrence</t>
+          <t>Số 5 Đường Nguyễn Huệ, TP Huế</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>710.534.2757</t>
+          <t>0901234104</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>Trần Dương</t>
+          <t>Phạm Thị I</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>Editor, commissioning</t>
+          <t>Nội trợ</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>754.873.4165x20820</t>
+          <t>091234514</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">
@@ -867,22 +867,22 @@
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>phạmquang15@gmail.com</t>
+          <t>ph14@gmail.com</t>
         </is>
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>Lê Quang</t>
+          <t>Phạm Thị J</t>
         </is>
       </c>
       <c r="L6" t="inlineStr">
         <is>
-          <t>Scientist, research (medical)</t>
+          <t>Nhân viên văn phòng</t>
         </is>
       </c>
       <c r="M6" t="inlineStr">
         <is>
-          <t>+1-831-782-6108x43088</t>
+          <t>098765414</t>
         </is>
       </c>
       <c r="N6" t="inlineStr">
@@ -892,126 +892,126 @@
       </c>
       <c r="O6" t="inlineStr">
         <is>
-          <t>trầnlinh67@gmail.com</t>
+          <t>ph24@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Bùi Vy</t>
+          <t>Nguyễn Văn F</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>08/05/2004</t>
+          <t>01/01/2015</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Nam</t>
+          <t>Nữ</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>79394 Wood Crossing, New Christineside</t>
+          <t>Số 6 Đường Nguyễn Huệ, TP Huế</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>015-452-2696x3417</t>
+          <t>0901234105</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>Bùi Bình</t>
+          <t>Phạm Thị K</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>Speech and language therapist</t>
+          <t>Nội trợ</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>(308)449-1717x045</t>
+          <t>091234515</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>Nữ</t>
+          <t>Nam</t>
         </is>
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>nguyễndương54@gmail.com</t>
+          <t>ph15@gmail.com</t>
         </is>
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>Phạm Khánh</t>
+          <t>Phạm Thị L</t>
         </is>
       </c>
       <c r="L7" t="inlineStr">
         <is>
-          <t>Recycling officer</t>
+          <t>Bác sĩ</t>
         </is>
       </c>
       <c r="M7" t="inlineStr">
         <is>
-          <t>723.224.1571x762</t>
+          <t>098765415</t>
         </is>
       </c>
       <c r="N7" t="inlineStr">
         <is>
-          <t>Nam</t>
+          <t>Nữ</t>
         </is>
       </c>
       <c r="O7" t="inlineStr">
         <is>
-          <t>nguyễnnam91@gmail.com</t>
+          <t>ph25@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Phạm Minh</t>
+          <t>Nguyễn Văn G</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>15/07/2006</t>
+          <t>01/01/2016</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Nữ</t>
+          <t>Nam</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>4728 Aaron Orchard, Nicholeville</t>
+          <t>Số 7 Đường Nguyễn Huệ, TP Huế</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>179-225-2744x96909</t>
+          <t>0901234106</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>Phan Minh</t>
+          <t>Phạm Thị M</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>Editorial assistant</t>
+          <t>Nhân viên văn phòng</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>(706)667-2307x844</t>
+          <t>091234516</t>
         </is>
       </c>
       <c r="I8" t="inlineStr">
@@ -1021,44 +1021,44 @@
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>lêvân92@gmail.com</t>
+          <t>ph16@gmail.com</t>
         </is>
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>Bùi Quang</t>
+          <t>Phạm Thị N</t>
         </is>
       </c>
       <c r="L8" t="inlineStr">
         <is>
-          <t>Garment/textile technologist</t>
+          <t>Nhân viên văn phòng</t>
         </is>
       </c>
       <c r="M8" t="inlineStr">
         <is>
-          <t>+1-685-157-9471x086</t>
+          <t>098765416</t>
         </is>
       </c>
       <c r="N8" t="inlineStr">
         <is>
-          <t>Nữ</t>
+          <t>Nam</t>
         </is>
       </c>
       <c r="O8" t="inlineStr">
         <is>
-          <t>phạmtú89@gmail.com</t>
+          <t>ph26@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Phan Hiền</t>
+          <t>Nguyễn Văn H</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>24/03/2006</t>
+          <t>01/01/2017</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -1068,27 +1068,27 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>299 Curtis Way, New Michelleton</t>
+          <t>Số 8 Đường Nguyễn Huệ, TP Huế</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>626-539-7581x44963</t>
+          <t>0901234107</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>Phạm Lan</t>
+          <t>Phạm Thị O</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>Tax inspector</t>
+          <t>Nội trợ</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>+1-727-373-6434</t>
+          <t>091234517</t>
         </is>
       </c>
       <c r="I9" t="inlineStr">
@@ -1098,44 +1098,44 @@
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>vũquang20@gmail.com</t>
+          <t>ph17@gmail.com</t>
         </is>
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>Nguyễn Hiền</t>
+          <t>Phạm Thị P</t>
         </is>
       </c>
       <c r="L9" t="inlineStr">
         <is>
-          <t>Facilities manager</t>
+          <t>Công nhân</t>
         </is>
       </c>
       <c r="M9" t="inlineStr">
         <is>
-          <t>567.691.3716x4730</t>
+          <t>098765417</t>
         </is>
       </c>
       <c r="N9" t="inlineStr">
         <is>
-          <t>Nam</t>
+          <t>Nữ</t>
         </is>
       </c>
       <c r="O9" t="inlineStr">
         <is>
-          <t>phạmbình65@gmail.com</t>
+          <t>ph27@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Vũ Phúc</t>
+          <t>Nguyễn Văn I</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>30/08/2005</t>
+          <t>01/01/2018</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -1145,74 +1145,74 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>353 Jack Overpass, Nancyville</t>
+          <t>Số 9 Đường Nguyễn Huệ, TP Huế</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>001-641-205-5817x857</t>
+          <t>0901234108</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>Hoàng Hải</t>
+          <t>Phạm Thị Q</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>Journalist, newspaper</t>
+          <t>Bác sĩ</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>082-365-4514</t>
+          <t>091234518</t>
         </is>
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>Nam</t>
+          <t>Nữ</t>
         </is>
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>trầnvy28@gmail.com</t>
+          <t>ph18@gmail.com</t>
         </is>
       </c>
       <c r="K10" t="inlineStr">
         <is>
-          <t>Vũ Vân</t>
+          <t>Phạm Thị R</t>
         </is>
       </c>
       <c r="L10" t="inlineStr">
         <is>
-          <t>Industrial/product designer</t>
+          <t>Nội trợ</t>
         </is>
       </c>
       <c r="M10" t="inlineStr">
         <is>
-          <t>256-392-2106x912</t>
+          <t>098765418</t>
         </is>
       </c>
       <c r="N10" t="inlineStr">
         <is>
-          <t>Nữ</t>
+          <t>Nam</t>
         </is>
       </c>
       <c r="O10" t="inlineStr">
         <is>
-          <t>đỗhiền9@gmail.com</t>
+          <t>ph28@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Trần Châu</t>
+          <t>Nguyễn Văn J</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>07/01/2003</t>
+          <t>01/01/2019</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -1222,52 +1222,52 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>424 Moran Flats, East Mitchell</t>
+          <t>Số 10 Đường Nguyễn Huệ, TP Huế</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>(642)832-8854x3948</t>
+          <t>0901234109</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>Nguyễn Hải</t>
+          <t>Phạm Thị S</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>Commercial/residential surveyor</t>
+          <t>Bác sĩ</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>375.384.6644x0258</t>
+          <t>091234519</t>
         </is>
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>Nữ</t>
+          <t>Nam</t>
         </is>
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>trầnhùng88@gmail.com</t>
+          <t>ph19@gmail.com</t>
         </is>
       </c>
       <c r="K11" t="inlineStr">
         <is>
-          <t>Vũ Quang</t>
+          <t>Phạm Thị T</t>
         </is>
       </c>
       <c r="L11" t="inlineStr">
         <is>
-          <t>Teacher, special educational needs</t>
+          <t>Kỹ sư</t>
         </is>
       </c>
       <c r="M11" t="inlineStr">
         <is>
-          <t>001-188-199-2399x959</t>
+          <t>098765419</t>
         </is>
       </c>
       <c r="N11" t="inlineStr">
@@ -1277,49 +1277,49 @@
       </c>
       <c r="O11" t="inlineStr">
         <is>
-          <t>phanphúc70@gmail.com</t>
+          <t>ph29@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Hoàng Nam</t>
+          <t>Nguyễn Văn K</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>03/08/2002</t>
+          <t>01/01/2010</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Nữ</t>
+          <t>Nam</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>388 Thomas Corner, Lake Michelleland</t>
+          <t>Số 11 Đường Nguyễn Huệ, TP Huế</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>001-276-251-6853x00094</t>
+          <t>0901234110</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>Vũ Hải</t>
+          <t>Phạm Thị U</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>Administrator, arts</t>
+          <t>Bác sĩ</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>777-320-8934x9937</t>
+          <t>091234520</t>
         </is>
       </c>
       <c r="I12" t="inlineStr">
@@ -1329,22 +1329,22 @@
       </c>
       <c r="J12" t="inlineStr">
         <is>
-          <t>phanvân27@gmail.com</t>
+          <t>ph110@gmail.com</t>
         </is>
       </c>
       <c r="K12" t="inlineStr">
         <is>
-          <t>Đặng Anh</t>
+          <t>Phạm Thị V</t>
         </is>
       </c>
       <c r="L12" t="inlineStr">
         <is>
-          <t>Archivist</t>
+          <t>Công nhân</t>
         </is>
       </c>
       <c r="M12" t="inlineStr">
         <is>
-          <t>001-235-820-8505x2189</t>
+          <t>098765420</t>
         </is>
       </c>
       <c r="N12" t="inlineStr">
@@ -1354,49 +1354,49 @@
       </c>
       <c r="O12" t="inlineStr">
         <is>
-          <t>đỗlan26@gmail.com</t>
+          <t>ph210@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Phan Vy</t>
+          <t>Nguyễn Văn L</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>29/10/2004</t>
+          <t>01/01/2011</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Nam</t>
+          <t>Nữ</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>34521 Jose Glens, West Joefurt</t>
+          <t>Số 12 Đường Nguyễn Huệ, TP Huế</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>400-662-3451x557</t>
+          <t>0901234111</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>Nguyễn Linh</t>
+          <t>Phạm Thị W</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>Surveyor, quantity</t>
+          <t>Giáo viên</t>
         </is>
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>+1-127-550-7816x42872</t>
+          <t>091234521</t>
         </is>
       </c>
       <c r="I13" t="inlineStr">
@@ -1406,74 +1406,74 @@
       </c>
       <c r="J13" t="inlineStr">
         <is>
-          <t>hoànganh60@gmail.com</t>
+          <t>ph111@gmail.com</t>
         </is>
       </c>
       <c r="K13" t="inlineStr">
         <is>
-          <t>Trần Tú</t>
+          <t>Phạm Thị X</t>
         </is>
       </c>
       <c r="L13" t="inlineStr">
         <is>
-          <t>Garment/textile technologist</t>
+          <t>Kỹ sư</t>
         </is>
       </c>
       <c r="M13" t="inlineStr">
         <is>
-          <t>696-209-4760</t>
+          <t>098765421</t>
         </is>
       </c>
       <c r="N13" t="inlineStr">
         <is>
-          <t>Nam</t>
+          <t>Nữ</t>
         </is>
       </c>
       <c r="O13" t="inlineStr">
         <is>
-          <t>lêanh56@gmail.com</t>
+          <t>ph211@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Hoàng Nam</t>
+          <t>Nguyễn Văn M</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>17/11/2006</t>
+          <t>01/01/2012</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Nữ</t>
+          <t>Nam</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>303 Mcdonald Stream, South Cindy</t>
+          <t>Số 13 Đường Nguyễn Huệ, TP Huế</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>2508742755</t>
+          <t>0901234112</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>Đặng Bình</t>
+          <t>Phạm Thị Y</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>Barista</t>
+          <t>Kỹ sư</t>
         </is>
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>(673)209-5719x01308</t>
+          <t>091234522</t>
         </is>
       </c>
       <c r="I14" t="inlineStr">
@@ -1483,22 +1483,22 @@
       </c>
       <c r="J14" t="inlineStr">
         <is>
-          <t>nguyễnnam63@gmail.com</t>
+          <t>ph112@gmail.com</t>
         </is>
       </c>
       <c r="K14" t="inlineStr">
         <is>
-          <t>Phạm Khánh</t>
+          <t>Phạm Thị Z</t>
         </is>
       </c>
       <c r="L14" t="inlineStr">
         <is>
-          <t>Teaching laboratory technician</t>
+          <t>Kỹ sư</t>
         </is>
       </c>
       <c r="M14" t="inlineStr">
         <is>
-          <t>(306)124-1745x397</t>
+          <t>098765422</t>
         </is>
       </c>
       <c r="N14" t="inlineStr">
@@ -1508,74 +1508,74 @@
       </c>
       <c r="O14" t="inlineStr">
         <is>
-          <t>vũphúc70@gmail.com</t>
+          <t>ph212@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Lê Khánh</t>
+          <t>Nguyễn Văn N</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>23/04/2007</t>
+          <t>01/01/2013</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Nam</t>
+          <t>Nữ</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>311 Miller Place, Gregoryland</t>
+          <t>Số 14 Đường Nguyễn Huệ, TP Huế</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>3191633569</t>
+          <t>0901234113</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>Vũ Linh</t>
+          <t>Phạm Thị [</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>Television camera operator</t>
+          <t>Nhân viên văn phòng</t>
         </is>
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>+1-147-171-9487</t>
+          <t>091234523</t>
         </is>
       </c>
       <c r="I15" t="inlineStr">
         <is>
-          <t>Nữ</t>
+          <t>Nam</t>
         </is>
       </c>
       <c r="J15" t="inlineStr">
         <is>
-          <t>trầnlinh33@gmail.com</t>
+          <t>ph113@gmail.com</t>
         </is>
       </c>
       <c r="K15" t="inlineStr">
         <is>
-          <t>Lê Hiền</t>
+          <t>Phạm Thị \</t>
         </is>
       </c>
       <c r="L15" t="inlineStr">
         <is>
-          <t>Scientist, research (life sciences)</t>
+          <t>Kỹ sư</t>
         </is>
       </c>
       <c r="M15" t="inlineStr">
         <is>
-          <t>(221)668-3953</t>
+          <t>098765423</t>
         </is>
       </c>
       <c r="N15" t="inlineStr">
@@ -1585,19 +1585,19 @@
       </c>
       <c r="O15" t="inlineStr">
         <is>
-          <t>nguyễnminh84@gmail.com</t>
+          <t>ph213@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Đặng Anh</t>
+          <t>Nguyễn Văn O</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>18/08/2001</t>
+          <t>01/01/2014</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
@@ -1607,27 +1607,27 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>43701 Brandon Run, Sandrabury</t>
+          <t>Số 15 Đường Nguyễn Huệ, TP Huế</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>+1-640-520-6415x4404</t>
+          <t>0901234114</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>Bùi Phúc</t>
+          <t>Phạm Thị ]</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>Surveyor, commercial/residential</t>
+          <t>Kỹ sư</t>
         </is>
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>969.382.2391x3838</t>
+          <t>091234524</t>
         </is>
       </c>
       <c r="I16" t="inlineStr">
@@ -1637,22 +1637,22 @@
       </c>
       <c r="J16" t="inlineStr">
         <is>
-          <t>đặngngọc53@gmail.com</t>
+          <t>ph114@gmail.com</t>
         </is>
       </c>
       <c r="K16" t="inlineStr">
         <is>
-          <t>Phan Trang</t>
+          <t>Phạm Thị ^</t>
         </is>
       </c>
       <c r="L16" t="inlineStr">
         <is>
-          <t>Operations geologist</t>
+          <t>Nội trợ</t>
         </is>
       </c>
       <c r="M16" t="inlineStr">
         <is>
-          <t>587.320.7002x937</t>
+          <t>098765424</t>
         </is>
       </c>
       <c r="N16" t="inlineStr">
@@ -1662,19 +1662,19 @@
       </c>
       <c r="O16" t="inlineStr">
         <is>
-          <t>đỗquang68@gmail.com</t>
+          <t>ph214@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Đặng Hùng</t>
+          <t>Nguyễn Văn P</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>08/08/2001</t>
+          <t>01/01/2015</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
@@ -1684,27 +1684,27 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>8501 Wilson Fields, Phillipsfurt</t>
+          <t>Số 16 Đường Nguyễn Huệ, TP Huế</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>001-353-495-0798</t>
+          <t>0901234115</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>Phạm Trang</t>
+          <t>Phạm Thị _</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>Public relations officer</t>
+          <t>Nội trợ</t>
         </is>
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>+1-912-932-0699x3675</t>
+          <t>091234525</t>
         </is>
       </c>
       <c r="I17" t="inlineStr">
@@ -1714,228 +1714,228 @@
       </c>
       <c r="J17" t="inlineStr">
         <is>
-          <t>hoàngvy17@gmail.com</t>
+          <t>ph115@gmail.com</t>
         </is>
       </c>
       <c r="K17" t="inlineStr">
         <is>
-          <t>Phạm Anh</t>
+          <t>Phạm Thị `</t>
         </is>
       </c>
       <c r="L17" t="inlineStr">
         <is>
-          <t>Sports development officer</t>
+          <t>Giáo viên</t>
         </is>
       </c>
       <c r="M17" t="inlineStr">
         <is>
-          <t>223-258-4554x177</t>
+          <t>098765425</t>
         </is>
       </c>
       <c r="N17" t="inlineStr">
         <is>
-          <t>Nam</t>
+          <t>Nữ</t>
         </is>
       </c>
       <c r="O17" t="inlineStr">
         <is>
-          <t>nguyễnvy15@gmail.com</t>
+          <t>ph215@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Vũ Bình</t>
+          <t>Nguyễn Văn Q</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>07/08/2003</t>
+          <t>01/01/2016</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Nữ</t>
+          <t>Nam</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>501 Tyler Motorway, Lake Danielmouth</t>
+          <t>Số 17 Đường Nguyễn Huệ, TP Huế</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>(651)502-9036</t>
+          <t>0901234116</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>Nguyễn Vân</t>
+          <t>Phạm Thị a</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>Information systems manager</t>
+          <t>Nhân viên văn phòng</t>
         </is>
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>933-710-9460</t>
+          <t>091234526</t>
         </is>
       </c>
       <c r="I18" t="inlineStr">
         <is>
-          <t>Nam</t>
+          <t>Nữ</t>
         </is>
       </c>
       <c r="J18" t="inlineStr">
         <is>
-          <t>bùilinh66@gmail.com</t>
+          <t>ph116@gmail.com</t>
         </is>
       </c>
       <c r="K18" t="inlineStr">
         <is>
-          <t>Đỗ Trang</t>
+          <t>Phạm Thị b</t>
         </is>
       </c>
       <c r="L18" t="inlineStr">
         <is>
-          <t>Furniture conservator/restorer</t>
+          <t>Bác sĩ</t>
         </is>
       </c>
       <c r="M18" t="inlineStr">
         <is>
-          <t>116-019-5715x31952</t>
+          <t>098765426</t>
         </is>
       </c>
       <c r="N18" t="inlineStr">
         <is>
-          <t>Nữ</t>
+          <t>Nam</t>
         </is>
       </c>
       <c r="O18" t="inlineStr">
         <is>
-          <t>trầnquang41@gmail.com</t>
+          <t>ph216@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Đỗ Hải</t>
+          <t>Nguyễn Văn R</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>27/12/2001</t>
+          <t>01/01/2017</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Nam</t>
+          <t>Nữ</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>2388 Matthew Plains, Knappfurt</t>
+          <t>Số 18 Đường Nguyễn Huệ, TP Huế</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>5032597647</t>
+          <t>0901234117</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>Phạm Bình</t>
+          <t>Phạm Thị c</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>Records manager</t>
+          <t>Giáo viên</t>
         </is>
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>083-301-4467</t>
+          <t>091234527</t>
         </is>
       </c>
       <c r="I19" t="inlineStr">
         <is>
-          <t>Nữ</t>
+          <t>Nam</t>
         </is>
       </c>
       <c r="J19" t="inlineStr">
         <is>
-          <t>nguyễnminh48@gmail.com</t>
+          <t>ph117@gmail.com</t>
         </is>
       </c>
       <c r="K19" t="inlineStr">
         <is>
-          <t>Phan Phúc</t>
+          <t>Phạm Thị d</t>
         </is>
       </c>
       <c r="L19" t="inlineStr">
         <is>
-          <t>Research scientist (maths)</t>
+          <t>Kỹ sư</t>
         </is>
       </c>
       <c r="M19" t="inlineStr">
         <is>
-          <t>001-199-690-4025x0756</t>
+          <t>098765427</t>
         </is>
       </c>
       <c r="N19" t="inlineStr">
         <is>
-          <t>Nam</t>
+          <t>Nữ</t>
         </is>
       </c>
       <c r="O19" t="inlineStr">
         <is>
-          <t>bùichâu89@gmail.com</t>
+          <t>ph217@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Bùi Quang</t>
+          <t>Nguyễn Văn S</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>27/07/2000</t>
+          <t>01/01/2018</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Nữ</t>
+          <t>Nam</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>68326 Gonzalez Heights, Sarahburgh</t>
+          <t>Số 19 Đường Nguyễn Huệ, TP Huế</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>(955)035-6896</t>
+          <t>0901234118</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>Phan Hải</t>
+          <t>Phạm Thị e</t>
         </is>
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>Private music teacher</t>
+          <t>Nội trợ</t>
         </is>
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>001-568-743-5003x63593</t>
+          <t>091234528</t>
         </is>
       </c>
       <c r="I20" t="inlineStr">
@@ -1945,22 +1945,22 @@
       </c>
       <c r="J20" t="inlineStr">
         <is>
-          <t>trầnbình7@gmail.com</t>
+          <t>ph118@gmail.com</t>
         </is>
       </c>
       <c r="K20" t="inlineStr">
         <is>
-          <t>Trần Trang</t>
+          <t>Phạm Thị f</t>
         </is>
       </c>
       <c r="L20" t="inlineStr">
         <is>
-          <t>Manufacturing engineer</t>
+          <t>Kỹ sư</t>
         </is>
       </c>
       <c r="M20" t="inlineStr">
         <is>
-          <t>(225)192-3757</t>
+          <t>098765428</t>
         </is>
       </c>
       <c r="N20" t="inlineStr">
@@ -1970,19 +1970,19 @@
       </c>
       <c r="O20" t="inlineStr">
         <is>
-          <t>hoàngnam35@gmail.com</t>
+          <t>ph218@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Trần Châu</t>
+          <t>Nguyễn Văn T</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>23/09/2002</t>
+          <t>01/01/2019</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
@@ -1992,27 +1992,27 @@
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>92336 Fisher Run, South Kristen</t>
+          <t>Số 20 Đường Nguyễn Huệ, TP Huế</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>(150)682-2387x0232</t>
+          <t>0901234119</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>Trần Vân</t>
+          <t>Phạm Thị g</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>Broadcast presenter</t>
+          <t>Nhân viên văn phòng</t>
         </is>
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>333-338-3633</t>
+          <t>091234529</t>
         </is>
       </c>
       <c r="I21" t="inlineStr">
@@ -2022,22 +2022,22 @@
       </c>
       <c r="J21" t="inlineStr">
         <is>
-          <t>lênam89@gmail.com</t>
+          <t>ph119@gmail.com</t>
         </is>
       </c>
       <c r="K21" t="inlineStr">
         <is>
-          <t>Đỗ Khánh</t>
+          <t>Phạm Thị h</t>
         </is>
       </c>
       <c r="L21" t="inlineStr">
         <is>
-          <t>Exercise physiologist</t>
+          <t>Công nhân</t>
         </is>
       </c>
       <c r="M21" t="inlineStr">
         <is>
-          <t>+1-369-188-0062x75706</t>
+          <t>098765429</t>
         </is>
       </c>
       <c r="N21" t="inlineStr">
@@ -2047,7 +2047,7 @@
       </c>
       <c r="O21" t="inlineStr">
         <is>
-          <t>hoàngdương6@gmail.com</t>
+          <t>ph219@gmail.com</t>
         </is>
       </c>
     </row>
@@ -2062,7 +2062,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I6"/>
+  <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2120,12 +2120,12 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Lê Ngọc</t>
+          <t>Trần Thị Mai</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>25/06/1992</t>
+          <t>12/05/1985</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -2135,22 +2135,22 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>178 Snyder Skyway, Jeffersonport</t>
+          <t>123 Lê Lợi, Đà Nẵng</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>001-190-666-1643</t>
+          <t>0911222333</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>lêngọc15@gmail.com</t>
+          <t>mai.tran@school.edu.vn</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>Research scientist (life sciences)</t>
+          <t>Toán</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
@@ -2159,18 +2159,18 @@
         </is>
       </c>
       <c r="I2" t="n">
-        <v>10</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Phan Linh</t>
+          <t>Lê Quốc Hùng</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>21/06/1987</t>
+          <t>23/11/1979</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -2180,22 +2180,22 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>28349 Jeremy Pine, Aliciaburgh</t>
+          <t>45 Nguyễn Trãi, TP HCM</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>+1-133-146-4815x81070</t>
+          <t>0933444555</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>phanlinh29@gmail.com</t>
+          <t>hung.le@school.edu.vn</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>Doctor, hospital</t>
+          <t>Văn</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
@@ -2204,142 +2204,7 @@
         </is>
       </c>
       <c r="I3" t="n">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>Trần Khánh</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>23/10/1995</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>Nam</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>450 Dodson Place, Smithbury</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>(074)218-0224x3816</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>trầnkhánh28@gmail.com</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>Proofreader</t>
-        </is>
-      </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>Tiến sĩ</t>
-        </is>
-      </c>
-      <c r="I4" t="n">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>Trần Trang</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>03/01/1992</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>Nam</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>7692 Christian Drive, East Kevin</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>+1-728-012-8475</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>trầntrang87@gmail.com</t>
-        </is>
-      </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>Chief Marketing Officer</t>
-        </is>
-      </c>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>Tiến sĩ</t>
-        </is>
-      </c>
-      <c r="I5" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>Vũ Minh</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>13/12/1996</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>Nữ</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>07857 Rojas Streets, Andersenmouth</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>(784)532-8624</t>
-        </is>
-      </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>vũminh7@gmail.com</t>
-        </is>
-      </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>Broadcast presenter</t>
-        </is>
-      </c>
-      <c r="H6" t="inlineStr">
-        <is>
-          <t>Cử nhân</t>
-        </is>
-      </c>
-      <c r="I6" t="n">
-        <v>8</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>